<commit_message>
Add order edit page and import to order
</commit_message>
<xml_diff>
--- a/public/import/catalog_import.xlsx
+++ b/public/import/catalog_import.xlsx
@@ -24,13 +24,13 @@
     <t>Артикул Dinmark</t>
   </si>
   <si>
-    <t>Ваш артикул внутри холдинга</t>
-  </si>
-  <si>
     <t>127-20цг</t>
   </si>
   <si>
     <t>127-20цг-холдинг</t>
+  </si>
+  <si>
+    <t>Артикул всередині холдингу</t>
   </si>
 </sst>
 </file>
@@ -362,7 +362,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -376,15 +376,15 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>